<commit_message>
Modified Edit User Profile
</commit_message>
<xml_diff>
--- a/Documents/ResourceControl.xlsx
+++ b/Documents/ResourceControl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="11480" windowHeight="3680"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="11480" windowHeight="3680" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ML" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="1074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="1077">
   <si>
     <t>Name</t>
   </si>
@@ -3241,6 +3241,15 @@
   </si>
   <si>
     <t>ML00209</t>
+  </si>
+  <si>
+    <t>Something went wrong. Please try again!</t>
+  </si>
+  <si>
+    <t>အမှားအယွင်းရှိနေ ပါသဖြည့် ပြန်လည် လုပ်ဆောင်ပါ။</t>
+  </si>
+  <si>
+    <t>MV00093</t>
   </si>
 </sst>
 </file>
@@ -3374,22 +3383,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -3401,6 +3395,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3708,7 +3717,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3717,8 +3726,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" style="12" customWidth="1"/>
     <col min="3" max="3" width="16.36328125" customWidth="1"/>
     <col min="4" max="4" width="57.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.81640625" customWidth="1"/>
@@ -3726,37 +3735,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>566</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="8" t="s">
         <v>1072</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -3767,10 +3776,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C4" t="s">
@@ -3784,10 +3793,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="12" t="s">
         <v>54</v>
       </c>
       <c r="C5" t="s">
@@ -3801,10 +3810,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C6" t="s">
@@ -3818,10 +3827,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C7" t="s">
@@ -3835,10 +3844,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="12" t="s">
         <v>59</v>
       </c>
       <c r="C8" t="s">
@@ -3852,10 +3861,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C9" t="s">
@@ -3869,10 +3878,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C10" t="s">
@@ -3886,10 +3895,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C11" t="s">
@@ -3903,10 +3912,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C12" t="s">
@@ -3920,10 +3929,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C13" t="s">
@@ -3937,10 +3946,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="12" t="s">
         <v>71</v>
       </c>
       <c r="C14" t="s">
@@ -3954,10 +3963,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
@@ -3971,10 +3980,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C16" t="s">
@@ -3988,10 +3997,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="12" t="s">
         <v>73</v>
       </c>
       <c r="C17" t="s">
@@ -4005,10 +4014,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="12" t="s">
         <v>74</v>
       </c>
       <c r="C18" t="s">
@@ -4022,10 +4031,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="12" t="s">
         <v>75</v>
       </c>
       <c r="C19" t="s">
@@ -4039,10 +4048,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="12" t="s">
         <v>76</v>
       </c>
       <c r="C20" t="s">
@@ -4056,10 +4065,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C21" t="s">
@@ -4073,10 +4082,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="12" t="s">
         <v>78</v>
       </c>
       <c r="C22" t="s">
@@ -4090,10 +4099,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="12" t="s">
         <v>79</v>
       </c>
       <c r="C23" t="s">
@@ -4107,10 +4116,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="12" t="s">
         <v>80</v>
       </c>
       <c r="C24" t="s">
@@ -4124,10 +4133,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="12" t="s">
         <v>81</v>
       </c>
       <c r="C25" t="s">
@@ -4141,10 +4150,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C26" t="s">
@@ -4158,10 +4167,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C27" t="s">
@@ -4175,10 +4184,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="12" t="s">
         <v>84</v>
       </c>
       <c r="C28" t="s">
@@ -4192,10 +4201,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="12" t="s">
         <v>85</v>
       </c>
       <c r="C29" t="s">
@@ -4209,10 +4218,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="12" t="s">
         <v>86</v>
       </c>
       <c r="C30" t="s">
@@ -4226,10 +4235,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="12" t="s">
         <v>87</v>
       </c>
       <c r="C31" t="s">
@@ -4243,10 +4252,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="12" t="s">
         <v>88</v>
       </c>
       <c r="C32" t="s">
@@ -4260,10 +4269,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="12" t="s">
         <v>89</v>
       </c>
       <c r="C33" t="s">
@@ -4277,10 +4286,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="12" t="s">
         <v>90</v>
       </c>
       <c r="C34" t="s">
@@ -4294,10 +4303,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="12" t="s">
         <v>91</v>
       </c>
       <c r="C35" t="s">
@@ -4311,10 +4320,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="12" t="s">
         <v>92</v>
       </c>
       <c r="C36" t="s">
@@ -4328,10 +4337,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C37" t="s">
@@ -4345,10 +4354,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="12" t="s">
         <v>93</v>
       </c>
       <c r="C38" t="s">
@@ -4362,10 +4371,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="12" t="s">
         <v>94</v>
       </c>
       <c r="C39" t="s">
@@ -4379,10 +4388,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="12" t="s">
         <v>95</v>
       </c>
       <c r="C40" t="s">
@@ -4396,10 +4405,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="12" t="s">
         <v>96</v>
       </c>
       <c r="C41" t="s">
@@ -4413,10 +4422,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C42" t="s">
@@ -4430,10 +4439,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="12" t="s">
         <v>98</v>
       </c>
       <c r="C43" t="s">
@@ -4447,10 +4456,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="12" t="s">
         <v>100</v>
       </c>
       <c r="C44" t="s">
@@ -4464,10 +4473,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="12" t="s">
         <v>101</v>
       </c>
       <c r="C45" t="s">
@@ -4481,10 +4490,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="12" t="s">
         <v>102</v>
       </c>
       <c r="C46" t="s">
@@ -4498,10 +4507,10 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C47" t="s">
@@ -4515,10 +4524,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="12" t="s">
         <v>104</v>
       </c>
       <c r="C48" t="s">
@@ -4532,10 +4541,10 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="12" t="s">
         <v>105</v>
       </c>
       <c r="C49" t="s">
@@ -4549,10 +4558,10 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="12" t="s">
         <v>106</v>
       </c>
       <c r="C50" t="s">
@@ -4566,10 +4575,10 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="12" t="s">
         <v>107</v>
       </c>
       <c r="C51" t="s">
@@ -4583,10 +4592,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="12" t="s">
         <v>108</v>
       </c>
       <c r="C52" t="s">
@@ -4600,10 +4609,10 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="12" t="s">
         <v>109</v>
       </c>
       <c r="C53" t="s">
@@ -4617,10 +4626,10 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="12" t="s">
         <v>110</v>
       </c>
       <c r="C54" t="s">
@@ -4634,10 +4643,10 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="12" t="s">
         <v>111</v>
       </c>
       <c r="C55" t="s">
@@ -4651,10 +4660,10 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="12" t="s">
         <v>112</v>
       </c>
       <c r="C56" t="s">
@@ -4668,10 +4677,10 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="12" t="s">
         <v>113</v>
       </c>
       <c r="C57" t="s">
@@ -4685,10 +4694,10 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="12" t="s">
         <v>114</v>
       </c>
       <c r="C58" t="s">
@@ -4702,10 +4711,10 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="12" t="s">
         <v>115</v>
       </c>
       <c r="C59" t="s">
@@ -4719,10 +4728,10 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="12" t="s">
         <v>116</v>
       </c>
       <c r="C60" t="s">
@@ -4736,10 +4745,10 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="12" t="s">
         <v>117</v>
       </c>
       <c r="C61" t="s">
@@ -4753,10 +4762,10 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="12" t="s">
         <v>118</v>
       </c>
       <c r="C62" t="s">
@@ -4770,10 +4779,10 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="12" t="s">
         <v>119</v>
       </c>
       <c r="C63" t="s">
@@ -4787,10 +4796,10 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="12" t="s">
         <v>120</v>
       </c>
       <c r="C64" t="s">
@@ -4804,10 +4813,10 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C65" t="s">
@@ -4821,10 +4830,10 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="12" t="s">
         <v>122</v>
       </c>
       <c r="C66" t="s">
@@ -4838,10 +4847,10 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="12" t="s">
         <v>123</v>
       </c>
       <c r="C67" t="s">
@@ -4855,10 +4864,10 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="16" t="s">
+      <c r="A68" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="12" t="s">
         <v>124</v>
       </c>
       <c r="C68" t="s">
@@ -4872,10 +4881,10 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="12" t="s">
         <v>125</v>
       </c>
       <c r="C69" t="s">
@@ -4889,10 +4898,10 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="16" t="s">
+      <c r="A70" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="12" t="s">
         <v>126</v>
       </c>
       <c r="C70" t="s">
@@ -4906,10 +4915,10 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="12" t="s">
         <v>127</v>
       </c>
       <c r="C71" t="s">
@@ -4923,10 +4932,10 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="16" t="s">
+      <c r="A72" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="12" t="s">
         <v>128</v>
       </c>
       <c r="C72" t="s">
@@ -4940,10 +4949,10 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="16" t="s">
+      <c r="A73" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="12" t="s">
         <v>129</v>
       </c>
       <c r="C73" t="s">
@@ -4957,10 +4966,10 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="12" t="s">
         <v>130</v>
       </c>
       <c r="C74" t="s">
@@ -4974,10 +4983,10 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="12" t="s">
         <v>131</v>
       </c>
       <c r="C75" t="s">
@@ -4991,10 +5000,10 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="12" t="s">
         <v>132</v>
       </c>
       <c r="C76" t="s">
@@ -5008,10 +5017,10 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" s="16" t="s">
+      <c r="A77" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="12" t="s">
         <v>204</v>
       </c>
       <c r="C77" t="s">
@@ -5025,10 +5034,10 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="16" t="s">
+      <c r="A78" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="12" t="s">
         <v>205</v>
       </c>
       <c r="C78" t="s">
@@ -5042,10 +5051,10 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" s="16" t="s">
+      <c r="A79" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="12" t="s">
         <v>206</v>
       </c>
       <c r="C79" t="s">
@@ -5059,10 +5068,10 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="16" t="s">
+      <c r="A80" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="12" t="s">
         <v>207</v>
       </c>
       <c r="C80" t="s">
@@ -5076,10 +5085,10 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="16" t="s">
+      <c r="A81" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="12" t="s">
         <v>208</v>
       </c>
       <c r="C81" t="s">
@@ -5093,10 +5102,10 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="16" t="s">
+      <c r="A82" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="B82" s="17" t="s">
+      <c r="B82" s="12" t="s">
         <v>209</v>
       </c>
       <c r="C82" t="s">
@@ -5110,10 +5119,10 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="16" t="s">
+      <c r="A83" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="12" t="s">
         <v>210</v>
       </c>
       <c r="C83" t="s">
@@ -5127,10 +5136,10 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="16" t="s">
+      <c r="A84" s="11" t="s">
         <v>586</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="B84" s="12" t="s">
         <v>961</v>
       </c>
       <c r="C84" t="s">
@@ -5144,10 +5153,10 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" s="16" t="s">
+      <c r="A85" s="11" t="s">
         <v>587</v>
       </c>
-      <c r="B85" s="17" t="s">
+      <c r="B85" s="12" t="s">
         <v>962</v>
       </c>
       <c r="C85" t="s">
@@ -5161,10 +5170,10 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" s="16" t="s">
+      <c r="A86" s="11" t="s">
         <v>588</v>
       </c>
-      <c r="B86" s="17" t="s">
+      <c r="B86" s="12" t="s">
         <v>963</v>
       </c>
       <c r="C86" t="s">
@@ -5178,10 +5187,10 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="16" t="s">
+      <c r="A87" s="11" t="s">
         <v>589</v>
       </c>
-      <c r="B87" s="17" t="s">
+      <c r="B87" s="12" t="s">
         <v>964</v>
       </c>
       <c r="C87" t="s">
@@ -5195,10 +5204,10 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="16" t="s">
+      <c r="A88" s="11" t="s">
         <v>590</v>
       </c>
-      <c r="B88" s="17" t="s">
+      <c r="B88" s="12" t="s">
         <v>551</v>
       </c>
       <c r="C88" t="s">
@@ -5212,10 +5221,10 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="16" t="s">
+      <c r="A89" s="11" t="s">
         <v>591</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="12" t="s">
         <v>552</v>
       </c>
       <c r="C89" t="s">
@@ -5229,10 +5238,10 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" s="16" t="s">
+      <c r="A90" s="11" t="s">
         <v>592</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="12" t="s">
         <v>553</v>
       </c>
       <c r="C90" t="s">
@@ -5246,10 +5255,10 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" s="16" t="s">
+      <c r="A91" s="11" t="s">
         <v>593</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="12" t="s">
         <v>556</v>
       </c>
       <c r="C91" t="s">
@@ -5263,10 +5272,10 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" s="16" t="s">
+      <c r="A92" s="11" t="s">
         <v>594</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="B92" s="12" t="s">
         <v>558</v>
       </c>
       <c r="C92" t="s">
@@ -5280,10 +5289,10 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" s="16" t="s">
+      <c r="A93" s="11" t="s">
         <v>595</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B93" s="12" t="s">
         <v>560</v>
       </c>
       <c r="C93" t="s">
@@ -5297,10 +5306,10 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="16" t="s">
+      <c r="A94" s="11" t="s">
         <v>596</v>
       </c>
-      <c r="B94" s="17" t="s">
+      <c r="B94" s="12" t="s">
         <v>562</v>
       </c>
       <c r="C94" t="s">
@@ -5314,10 +5323,10 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="16" t="s">
+      <c r="A95" s="11" t="s">
         <v>597</v>
       </c>
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="12" t="s">
         <v>564</v>
       </c>
       <c r="C95" t="s">
@@ -5331,10 +5340,10 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" s="16" t="s">
+      <c r="A96" s="11" t="s">
         <v>598</v>
       </c>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="12" t="s">
         <v>572</v>
       </c>
       <c r="C96" t="s">
@@ -5348,10 +5357,10 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97" s="16" t="s">
+      <c r="A97" s="11" t="s">
         <v>599</v>
       </c>
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="12" t="s">
         <v>574</v>
       </c>
       <c r="C97" t="s">
@@ -5365,10 +5374,10 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A98" s="16" t="s">
+      <c r="A98" s="11" t="s">
         <v>600</v>
       </c>
-      <c r="B98" s="17" t="s">
+      <c r="B98" s="12" t="s">
         <v>576</v>
       </c>
       <c r="C98" t="s">
@@ -5382,10 +5391,10 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A99" s="16" t="s">
+      <c r="A99" s="11" t="s">
         <v>601</v>
       </c>
-      <c r="B99" s="17" t="s">
+      <c r="B99" s="12" t="s">
         <v>578</v>
       </c>
       <c r="C99" t="s">
@@ -5399,10 +5408,10 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100" s="16" t="s">
+      <c r="A100" s="11" t="s">
         <v>602</v>
       </c>
-      <c r="B100" s="18" t="s">
+      <c r="B100" s="13" t="s">
         <v>580</v>
       </c>
       <c r="C100" t="s">
@@ -5416,10 +5425,10 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A101" s="16" t="s">
+      <c r="A101" s="11" t="s">
         <v>603</v>
       </c>
-      <c r="B101" s="17" t="s">
+      <c r="B101" s="12" t="s">
         <v>582</v>
       </c>
       <c r="C101" t="s">
@@ -5433,10 +5442,10 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A102" s="16" t="s">
+      <c r="A102" s="11" t="s">
         <v>613</v>
       </c>
-      <c r="B102" s="17" t="s">
+      <c r="B102" s="12" t="s">
         <v>611</v>
       </c>
       <c r="C102" t="s">
@@ -5450,10 +5459,10 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" s="16" t="s">
+      <c r="A103" s="11" t="s">
         <v>616</v>
       </c>
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="12" t="s">
         <v>614</v>
       </c>
       <c r="C103" t="s">
@@ -5467,10 +5476,10 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104" s="16" t="s">
+      <c r="A104" s="11" t="s">
         <v>617</v>
       </c>
-      <c r="B104" s="17" t="s">
+      <c r="B104" s="12" t="s">
         <v>615</v>
       </c>
       <c r="C104" t="s">
@@ -5484,10 +5493,10 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A105" s="16" t="s">
+      <c r="A105" s="11" t="s">
         <v>618</v>
       </c>
-      <c r="B105" s="17" t="s">
+      <c r="B105" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C105" t="s">
@@ -5501,10 +5510,10 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A106" s="16" t="s">
+      <c r="A106" s="11" t="s">
         <v>621</v>
       </c>
-      <c r="B106" s="17" t="s">
+      <c r="B106" s="12" t="s">
         <v>619</v>
       </c>
       <c r="C106" t="s">
@@ -5518,10 +5527,10 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A107" s="16" t="s">
+      <c r="A107" s="11" t="s">
         <v>622</v>
       </c>
-      <c r="B107" s="17" t="s">
+      <c r="B107" s="12" t="s">
         <v>620</v>
       </c>
       <c r="C107" t="s">
@@ -5535,10 +5544,10 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108" s="16" t="s">
+      <c r="A108" s="11" t="s">
         <v>641</v>
       </c>
-      <c r="B108" s="17" t="s">
+      <c r="B108" s="12" t="s">
         <v>625</v>
       </c>
       <c r="C108" t="s">
@@ -5552,10 +5561,10 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A109" s="16" t="s">
+      <c r="A109" s="11" t="s">
         <v>642</v>
       </c>
-      <c r="B109" s="17" t="s">
+      <c r="B109" s="12" t="s">
         <v>626</v>
       </c>
       <c r="C109" t="s">
@@ -5569,10 +5578,10 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A110" s="16" t="s">
+      <c r="A110" s="11" t="s">
         <v>643</v>
       </c>
-      <c r="B110" s="17" t="s">
+      <c r="B110" s="12" t="s">
         <v>627</v>
       </c>
       <c r="C110" t="s">
@@ -5586,10 +5595,10 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A111" s="16" t="s">
+      <c r="A111" s="11" t="s">
         <v>644</v>
       </c>
-      <c r="B111" s="17" t="s">
+      <c r="B111" s="12" t="s">
         <v>628</v>
       </c>
       <c r="C111" t="s">
@@ -5603,10 +5612,10 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A112" s="16" t="s">
+      <c r="A112" s="11" t="s">
         <v>645</v>
       </c>
-      <c r="B112" s="17" t="s">
+      <c r="B112" s="12" t="s">
         <v>629</v>
       </c>
       <c r="C112" t="s">
@@ -5620,10 +5629,10 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A113" s="16" t="s">
+      <c r="A113" s="11" t="s">
         <v>646</v>
       </c>
-      <c r="B113" s="17" t="s">
+      <c r="B113" s="12" t="s">
         <v>630</v>
       </c>
       <c r="C113" t="s">
@@ -5637,10 +5646,10 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A114" s="16" t="s">
+      <c r="A114" s="11" t="s">
         <v>647</v>
       </c>
-      <c r="B114" s="17" t="s">
+      <c r="B114" s="12" t="s">
         <v>631</v>
       </c>
       <c r="C114" t="s">
@@ -5654,10 +5663,10 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A115" s="16" t="s">
+      <c r="A115" s="11" t="s">
         <v>648</v>
       </c>
-      <c r="B115" s="17" t="s">
+      <c r="B115" s="12" t="s">
         <v>632</v>
       </c>
       <c r="C115" t="s">
@@ -5671,10 +5680,10 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A116" s="16" t="s">
+      <c r="A116" s="11" t="s">
         <v>649</v>
       </c>
-      <c r="B116" s="17" t="s">
+      <c r="B116" s="12" t="s">
         <v>633</v>
       </c>
       <c r="C116" t="s">
@@ -5688,10 +5697,10 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A117" s="16" t="s">
+      <c r="A117" s="11" t="s">
         <v>658</v>
       </c>
-      <c r="B117" s="17" t="s">
+      <c r="B117" s="12" t="s">
         <v>652</v>
       </c>
       <c r="C117" t="s">
@@ -5705,10 +5714,10 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A118" s="16" t="s">
+      <c r="A118" s="11" t="s">
         <v>659</v>
       </c>
-      <c r="B118" s="17" t="s">
+      <c r="B118" s="12" t="s">
         <v>654</v>
       </c>
       <c r="C118" t="s">
@@ -5722,10 +5731,10 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A119" s="16" t="s">
+      <c r="A119" s="11" t="s">
         <v>660</v>
       </c>
-      <c r="B119" s="17" t="s">
+      <c r="B119" s="12" t="s">
         <v>655</v>
       </c>
       <c r="C119" t="s">
@@ -5739,10 +5748,10 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A120" s="16" t="s">
+      <c r="A120" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="B120" s="17" t="s">
+      <c r="B120" s="12" t="s">
         <v>670</v>
       </c>
       <c r="C120" t="s">
@@ -5756,10 +5765,10 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="16" t="s">
+      <c r="A121" s="11" t="s">
         <v>675</v>
       </c>
-      <c r="B121" s="17" t="s">
+      <c r="B121" s="12" t="s">
         <v>671</v>
       </c>
       <c r="C121" t="s">
@@ -5773,10 +5782,10 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A122" s="16" t="s">
+      <c r="A122" s="11" t="s">
         <v>680</v>
       </c>
-      <c r="B122" s="17" t="s">
+      <c r="B122" s="12" t="s">
         <v>676</v>
       </c>
       <c r="C122" t="s">
@@ -5790,10 +5799,10 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A123" s="16" t="s">
+      <c r="A123" s="11" t="s">
         <v>681</v>
       </c>
-      <c r="B123" s="17" t="s">
+      <c r="B123" s="12" t="s">
         <v>677</v>
       </c>
       <c r="C123" t="s">
@@ -5807,10 +5816,10 @@
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A124" s="16" t="s">
+      <c r="A124" s="11" t="s">
         <v>682</v>
       </c>
-      <c r="B124" s="17" t="s">
+      <c r="B124" s="12" t="s">
         <v>683</v>
       </c>
       <c r="C124" t="s">
@@ -5824,10 +5833,10 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A125" s="16" t="s">
+      <c r="A125" s="11" t="s">
         <v>685</v>
       </c>
-      <c r="B125" s="17" t="s">
+      <c r="B125" s="12" t="s">
         <v>684</v>
       </c>
       <c r="C125" t="s">
@@ -5841,10 +5850,10 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A126" s="16" t="s">
+      <c r="A126" s="11" t="s">
         <v>688</v>
       </c>
-      <c r="B126" s="17" t="s">
+      <c r="B126" s="12" t="s">
         <v>686</v>
       </c>
       <c r="C126" t="s">
@@ -5858,10 +5867,10 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A127" s="16" t="s">
+      <c r="A127" s="11" t="s">
         <v>689</v>
       </c>
-      <c r="B127" s="17" t="s">
+      <c r="B127" s="12" t="s">
         <v>687</v>
       </c>
       <c r="C127" t="s">
@@ -5875,10 +5884,10 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A128" s="16" t="s">
+      <c r="A128" s="11" t="s">
         <v>692</v>
       </c>
-      <c r="B128" s="17" t="s">
+      <c r="B128" s="12" t="s">
         <v>113</v>
       </c>
       <c r="C128" t="s">
@@ -5892,10 +5901,10 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A129" s="16" t="s">
+      <c r="A129" s="11" t="s">
         <v>695</v>
       </c>
-      <c r="B129" s="17" t="s">
+      <c r="B129" s="12" t="s">
         <v>694</v>
       </c>
       <c r="C129" t="s">
@@ -5909,10 +5918,10 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A130" s="16" t="s">
+      <c r="A130" s="11" t="s">
         <v>699</v>
       </c>
-      <c r="B130" s="17" t="s">
+      <c r="B130" s="12" t="s">
         <v>697</v>
       </c>
       <c r="C130" t="s">
@@ -5926,10 +5935,10 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A131" s="16" t="s">
+      <c r="A131" s="11" t="s">
         <v>700</v>
       </c>
-      <c r="B131" s="17" t="s">
+      <c r="B131" s="12" t="s">
         <v>552</v>
       </c>
       <c r="C131" t="s">
@@ -5943,10 +5952,10 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A132" s="16" t="s">
+      <c r="A132" s="11" t="s">
         <v>704</v>
       </c>
-      <c r="B132" s="17" t="s">
+      <c r="B132" s="12" t="s">
         <v>582</v>
       </c>
       <c r="C132" t="s">
@@ -5960,10 +5969,10 @@
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A133" s="16" t="s">
+      <c r="A133" s="11" t="s">
         <v>705</v>
       </c>
-      <c r="B133" s="17" t="s">
+      <c r="B133" s="12" t="s">
         <v>702</v>
       </c>
       <c r="C133" t="s">
@@ -5977,10 +5986,10 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A134" s="16" t="s">
+      <c r="A134" s="11" t="s">
         <v>706</v>
       </c>
-      <c r="B134" s="17" t="s">
+      <c r="B134" s="12" t="s">
         <v>580</v>
       </c>
       <c r="C134" t="s">
@@ -5994,10 +6003,10 @@
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A135" s="16" t="s">
+      <c r="A135" s="11" t="s">
         <v>713</v>
       </c>
-      <c r="B135" s="19" t="s">
+      <c r="B135" s="14" t="s">
         <v>707</v>
       </c>
       <c r="C135" t="s">
@@ -6011,10 +6020,10 @@
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A136" s="16" t="s">
+      <c r="A136" s="11" t="s">
         <v>714</v>
       </c>
-      <c r="B136" s="17" t="s">
+      <c r="B136" s="12" t="s">
         <v>709</v>
       </c>
       <c r="C136" t="s">
@@ -6028,10 +6037,10 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A137" s="16" t="s">
+      <c r="A137" s="11" t="s">
         <v>715</v>
       </c>
-      <c r="B137" s="17" t="s">
+      <c r="B137" s="12" t="s">
         <v>711</v>
       </c>
       <c r="C137" t="s">
@@ -6045,10 +6054,10 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A138" s="16" t="s">
+      <c r="A138" s="11" t="s">
         <v>721</v>
       </c>
-      <c r="B138" s="17" t="s">
+      <c r="B138" s="12" t="s">
         <v>719</v>
       </c>
       <c r="C138" t="s">
@@ -6062,10 +6071,10 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A139" s="16" t="s">
+      <c r="A139" s="11" t="s">
         <v>724</v>
       </c>
-      <c r="B139" s="17" t="s">
+      <c r="B139" s="12" t="s">
         <v>722</v>
       </c>
       <c r="C139" t="s">
@@ -6079,10 +6088,10 @@
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A140" s="16" t="s">
+      <c r="A140" s="11" t="s">
         <v>780</v>
       </c>
-      <c r="B140" s="17" t="s">
+      <c r="B140" s="12" t="s">
         <v>762</v>
       </c>
       <c r="C140" t="s">
@@ -6102,10 +6111,10 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A141" s="16" t="s">
+      <c r="A141" s="11" t="s">
         <v>781</v>
       </c>
-      <c r="B141" s="17" t="s">
+      <c r="B141" s="12" t="s">
         <v>763</v>
       </c>
       <c r="C141" t="s">
@@ -6125,10 +6134,10 @@
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A142" s="16" t="s">
+      <c r="A142" s="11" t="s">
         <v>782</v>
       </c>
-      <c r="B142" s="17" t="s">
+      <c r="B142" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C142" t="s">
@@ -6148,10 +6157,10 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A143" s="16" t="s">
+      <c r="A143" s="11" t="s">
         <v>783</v>
       </c>
-      <c r="B143" s="17" t="s">
+      <c r="B143" s="12" t="s">
         <v>764</v>
       </c>
       <c r="C143" t="s">
@@ -6171,10 +6180,10 @@
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A144" s="16" t="s">
+      <c r="A144" s="11" t="s">
         <v>784</v>
       </c>
-      <c r="B144" s="17" t="s">
+      <c r="B144" s="12" t="s">
         <v>765</v>
       </c>
       <c r="C144" t="s">
@@ -6194,10 +6203,10 @@
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A145" s="16" t="s">
+      <c r="A145" s="11" t="s">
         <v>785</v>
       </c>
-      <c r="B145" s="17" t="s">
+      <c r="B145" s="12" t="s">
         <v>766</v>
       </c>
       <c r="C145" t="s">
@@ -6217,10 +6226,10 @@
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A146" s="16" t="s">
+      <c r="A146" s="11" t="s">
         <v>786</v>
       </c>
-      <c r="B146" s="17" t="s">
+      <c r="B146" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C146" t="s">
@@ -6240,10 +6249,10 @@
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A147" s="16" t="s">
+      <c r="A147" s="11" t="s">
         <v>787</v>
       </c>
-      <c r="B147" s="20" t="s">
+      <c r="B147" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C147" t="s">
@@ -6263,10 +6272,10 @@
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A148" s="16" t="s">
+      <c r="A148" s="11" t="s">
         <v>788</v>
       </c>
-      <c r="B148" s="17" t="s">
+      <c r="B148" s="12" t="s">
         <v>767</v>
       </c>
       <c r="C148" t="s">
@@ -6286,10 +6295,10 @@
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A149" s="16" t="s">
+      <c r="A149" s="11" t="s">
         <v>789</v>
       </c>
-      <c r="B149" s="17" t="s">
+      <c r="B149" s="12" t="s">
         <v>768</v>
       </c>
       <c r="C149" t="s">
@@ -6309,10 +6318,10 @@
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A150" s="16" t="s">
+      <c r="A150" s="11" t="s">
         <v>790</v>
       </c>
-      <c r="B150" s="20" t="s">
+      <c r="B150" s="15" t="s">
         <v>757</v>
       </c>
       <c r="C150" t="s">
@@ -6332,10 +6341,10 @@
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A151" s="16" t="s">
+      <c r="A151" s="11" t="s">
         <v>791</v>
       </c>
-      <c r="B151" s="20" t="s">
+      <c r="B151" s="15" t="s">
         <v>758</v>
       </c>
       <c r="C151" t="s">
@@ -6355,10 +6364,10 @@
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A152" s="16" t="s">
+      <c r="A152" s="11" t="s">
         <v>792</v>
       </c>
-      <c r="B152" s="20" t="s">
+      <c r="B152" s="15" t="s">
         <v>759</v>
       </c>
       <c r="C152" t="s">
@@ -6378,10 +6387,10 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A153" s="16" t="s">
+      <c r="A153" s="11" t="s">
         <v>793</v>
       </c>
-      <c r="B153" s="17" t="s">
+      <c r="B153" s="12" t="s">
         <v>760</v>
       </c>
       <c r="C153" t="s">
@@ -6401,10 +6410,10 @@
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A154" s="16" t="s">
+      <c r="A154" s="11" t="s">
         <v>794</v>
       </c>
-      <c r="B154" s="17" t="s">
+      <c r="B154" s="12" t="s">
         <v>761</v>
       </c>
       <c r="C154" t="s">
@@ -6424,10 +6433,10 @@
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A155" s="16" t="s">
+      <c r="A155" s="11" t="s">
         <v>807</v>
       </c>
-      <c r="B155" s="17" t="s">
+      <c r="B155" s="12" t="s">
         <v>795</v>
       </c>
       <c r="C155" t="s">
@@ -6447,10 +6456,10 @@
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A156" s="16" t="s">
+      <c r="A156" s="11" t="s">
         <v>808</v>
       </c>
-      <c r="B156" s="17" t="s">
+      <c r="B156" s="12" t="s">
         <v>796</v>
       </c>
       <c r="C156" t="s">
@@ -6470,10 +6479,10 @@
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A157" s="16" t="s">
+      <c r="A157" s="11" t="s">
         <v>809</v>
       </c>
-      <c r="B157" s="17" t="s">
+      <c r="B157" s="12" t="s">
         <v>797</v>
       </c>
       <c r="C157" t="s">
@@ -6493,10 +6502,10 @@
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A158" s="16" t="s">
+      <c r="A158" s="11" t="s">
         <v>815</v>
       </c>
-      <c r="B158" s="17" t="s">
+      <c r="B158" s="12" t="s">
         <v>814</v>
       </c>
       <c r="C158" t="s">
@@ -6516,10 +6525,10 @@
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A159" s="16" t="s">
+      <c r="A159" s="11" t="s">
         <v>834</v>
       </c>
-      <c r="B159" s="17" t="s">
+      <c r="B159" s="12" t="s">
         <v>832</v>
       </c>
       <c r="C159" t="s">
@@ -6539,10 +6548,10 @@
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A160" s="16" t="s">
+      <c r="A160" s="11" t="s">
         <v>837</v>
       </c>
-      <c r="B160" s="17" t="s">
+      <c r="B160" s="12" t="s">
         <v>836</v>
       </c>
       <c r="C160" t="s">
@@ -6562,10 +6571,10 @@
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A161" s="16" t="s">
+      <c r="A161" s="11" t="s">
         <v>840</v>
       </c>
-      <c r="B161" s="17" t="s">
+      <c r="B161" s="12" t="s">
         <v>838</v>
       </c>
       <c r="C161" t="s">
@@ -6585,10 +6594,10 @@
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A162" s="16" t="s">
+      <c r="A162" s="11" t="s">
         <v>843</v>
       </c>
-      <c r="B162" s="17" t="s">
+      <c r="B162" s="12" t="s">
         <v>841</v>
       </c>
       <c r="C162" t="s">
@@ -6608,10 +6617,10 @@
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A163" s="16" t="s">
+      <c r="A163" s="11" t="s">
         <v>845</v>
       </c>
-      <c r="B163" s="17" t="s">
+      <c r="B163" s="12" t="s">
         <v>844</v>
       </c>
       <c r="C163" t="s">
@@ -6631,10 +6640,10 @@
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A164" s="16" t="s">
+      <c r="A164" s="11" t="s">
         <v>849</v>
       </c>
-      <c r="B164" s="17" t="s">
+      <c r="B164" s="12" t="s">
         <v>846</v>
       </c>
       <c r="C164" t="s">
@@ -6654,10 +6663,10 @@
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A165" s="16" t="s">
+      <c r="A165" s="11" t="s">
         <v>851</v>
       </c>
-      <c r="B165" s="17" t="s">
+      <c r="B165" s="12" t="s">
         <v>850</v>
       </c>
       <c r="C165" t="s">
@@ -6677,10 +6686,10 @@
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A166" s="16" t="s">
+      <c r="A166" s="11" t="s">
         <v>854</v>
       </c>
-      <c r="B166" s="17" t="s">
+      <c r="B166" s="12" t="s">
         <v>852</v>
       </c>
       <c r="C166" t="s">
@@ -6700,10 +6709,10 @@
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A167" s="16" t="s">
+      <c r="A167" s="11" t="s">
         <v>861</v>
       </c>
-      <c r="B167" s="17" t="s">
+      <c r="B167" s="12" t="s">
         <v>855</v>
       </c>
       <c r="C167" t="s">
@@ -6723,10 +6732,10 @@
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A168" s="16" t="s">
+      <c r="A168" s="11" t="s">
         <v>862</v>
       </c>
-      <c r="B168" s="17" t="s">
+      <c r="B168" s="12" t="s">
         <v>856</v>
       </c>
       <c r="C168" t="s">
@@ -6746,10 +6755,10 @@
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A169" s="16" t="s">
+      <c r="A169" s="11" t="s">
         <v>863</v>
       </c>
-      <c r="B169" s="17" t="s">
+      <c r="B169" s="12" t="s">
         <v>857</v>
       </c>
       <c r="C169" t="s">
@@ -6769,10 +6778,10 @@
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A170" s="16" t="s">
+      <c r="A170" s="11" t="s">
         <v>866</v>
       </c>
-      <c r="B170" s="17" t="s">
+      <c r="B170" s="12" t="s">
         <v>864</v>
       </c>
       <c r="C170" t="s">
@@ -6792,10 +6801,10 @@
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A171" s="16" t="s">
+      <c r="A171" s="11" t="s">
         <v>869</v>
       </c>
-      <c r="B171" s="17" t="s">
+      <c r="B171" s="12" t="s">
         <v>867</v>
       </c>
       <c r="C171" t="s">
@@ -6815,10 +6824,10 @@
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A172" s="16" t="s">
+      <c r="A172" s="11" t="s">
         <v>872</v>
       </c>
-      <c r="B172" s="17" t="s">
+      <c r="B172" s="12" t="s">
         <v>870</v>
       </c>
       <c r="C172" t="s">
@@ -6838,10 +6847,10 @@
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A173" s="16" t="s">
+      <c r="A173" s="11" t="s">
         <v>874</v>
       </c>
-      <c r="B173" s="17" t="s">
+      <c r="B173" s="12" t="s">
         <v>876</v>
       </c>
       <c r="C173" t="s">
@@ -6861,10 +6870,10 @@
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A174" s="16" t="s">
+      <c r="A174" s="11" t="s">
         <v>878</v>
       </c>
-      <c r="B174" s="17" t="s">
+      <c r="B174" s="12" t="s">
         <v>875</v>
       </c>
       <c r="C174" t="s">
@@ -6884,10 +6893,10 @@
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A175" s="16" t="s">
+      <c r="A175" s="11" t="s">
         <v>881</v>
       </c>
-      <c r="B175" s="17" t="s">
+      <c r="B175" s="12" t="s">
         <v>879</v>
       </c>
       <c r="C175" t="s">
@@ -6907,10 +6916,10 @@
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A176" s="16" t="s">
+      <c r="A176" s="11" t="s">
         <v>884</v>
       </c>
-      <c r="B176" s="17" t="s">
+      <c r="B176" s="12" t="s">
         <v>882</v>
       </c>
       <c r="C176" t="s">
@@ -6930,10 +6939,10 @@
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A177" s="16" t="s">
+      <c r="A177" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="B177" s="17" t="s">
+      <c r="B177" s="12" t="s">
         <v>900</v>
       </c>
       <c r="C177" t="s">
@@ -6953,10 +6962,10 @@
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A178" s="16" t="s">
+      <c r="A178" s="11" t="s">
         <v>904</v>
       </c>
-      <c r="B178" s="17" t="s">
+      <c r="B178" s="12" t="s">
         <v>905</v>
       </c>
       <c r="C178" t="s">
@@ -6976,10 +6985,10 @@
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A179" s="16" t="s">
+      <c r="A179" s="11" t="s">
         <v>914</v>
       </c>
-      <c r="B179" s="17" t="s">
+      <c r="B179" s="12" t="s">
         <v>913</v>
       </c>
       <c r="C179" t="s">
@@ -6999,10 +7008,10 @@
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A180" s="16" t="s">
+      <c r="A180" s="11" t="s">
         <v>950</v>
       </c>
-      <c r="B180" s="17" t="s">
+      <c r="B180" s="12" t="s">
         <v>948</v>
       </c>
       <c r="C180" t="s">
@@ -7022,10 +7031,10 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A181" s="16" t="s">
+      <c r="A181" s="11" t="s">
         <v>960</v>
       </c>
-      <c r="B181" s="17" t="s">
+      <c r="B181" s="12" t="s">
         <v>958</v>
       </c>
       <c r="C181" t="s">
@@ -7045,10 +7054,10 @@
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A182" s="16" t="s">
+      <c r="A182" s="11" t="s">
         <v>969</v>
       </c>
-      <c r="B182" s="17" t="s">
+      <c r="B182" s="12" t="s">
         <v>965</v>
       </c>
       <c r="C182" t="s">
@@ -7068,10 +7077,10 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A183" s="16" t="s">
+      <c r="A183" s="11" t="s">
         <v>970</v>
       </c>
-      <c r="B183" s="17" t="s">
+      <c r="B183" s="12" t="s">
         <v>967</v>
       </c>
       <c r="C183" t="s">
@@ -7091,10 +7100,10 @@
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A184" s="16" t="s">
+      <c r="A184" s="11" t="s">
         <v>983</v>
       </c>
-      <c r="B184" s="17" t="s">
+      <c r="B184" s="12" t="s">
         <v>974</v>
       </c>
       <c r="C184" t="s">
@@ -7114,10 +7123,10 @@
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A185" s="16" t="s">
+      <c r="A185" s="11" t="s">
         <v>984</v>
       </c>
-      <c r="B185" s="17" t="s">
+      <c r="B185" s="12" t="s">
         <v>975</v>
       </c>
       <c r="C185" t="s">
@@ -7137,10 +7146,10 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A186" s="16" t="s">
+      <c r="A186" s="11" t="s">
         <v>985</v>
       </c>
-      <c r="B186" s="17" t="s">
+      <c r="B186" s="12" t="s">
         <v>976</v>
       </c>
       <c r="C186" t="s">
@@ -7160,10 +7169,10 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A187" s="16" t="s">
+      <c r="A187" s="11" t="s">
         <v>986</v>
       </c>
-      <c r="B187" s="17" t="s">
+      <c r="B187" s="12" t="s">
         <v>977</v>
       </c>
       <c r="C187" t="s">
@@ -7183,10 +7192,10 @@
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A188" s="16" t="s">
+      <c r="A188" s="11" t="s">
         <v>987</v>
       </c>
-      <c r="B188" s="17" t="s">
+      <c r="B188" s="12" t="s">
         <v>978</v>
       </c>
       <c r="C188" t="s">
@@ -7206,10 +7215,10 @@
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A189" s="16" t="s">
+      <c r="A189" s="11" t="s">
         <v>988</v>
       </c>
-      <c r="B189" s="17" t="s">
+      <c r="B189" s="12" t="s">
         <v>979</v>
       </c>
       <c r="C189" t="s">
@@ -7229,10 +7238,10 @@
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A190" s="16" t="s">
+      <c r="A190" s="11" t="s">
         <v>989</v>
       </c>
-      <c r="B190" s="17" t="s">
+      <c r="B190" s="12" t="s">
         <v>980</v>
       </c>
       <c r="C190" t="s">
@@ -7252,10 +7261,10 @@
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A191" s="16" t="s">
+      <c r="A191" s="11" t="s">
         <v>990</v>
       </c>
-      <c r="B191" s="17" t="s">
+      <c r="B191" s="12" t="s">
         <v>981</v>
       </c>
       <c r="C191" t="s">
@@ -7275,10 +7284,10 @@
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A192" s="16" t="s">
+      <c r="A192" s="11" t="s">
         <v>991</v>
       </c>
-      <c r="B192" s="17" t="s">
+      <c r="B192" s="12" t="s">
         <v>982</v>
       </c>
       <c r="C192" t="s">
@@ -7298,10 +7307,10 @@
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A193" s="16" t="s">
+      <c r="A193" s="11" t="s">
         <v>1016</v>
       </c>
-      <c r="B193" s="17" t="s">
+      <c r="B193" s="12" t="s">
         <v>1014</v>
       </c>
       <c r="C193" t="s">
@@ -7315,10 +7324,10 @@
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A194" s="16" t="s">
+      <c r="A194" s="11" t="s">
         <v>1033</v>
       </c>
-      <c r="B194" s="17" t="s">
+      <c r="B194" s="12" t="s">
         <v>1017</v>
       </c>
       <c r="C194" t="s">
@@ -7338,10 +7347,10 @@
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A195" s="16" t="s">
+      <c r="A195" s="11" t="s">
         <v>1034</v>
       </c>
-      <c r="B195" s="17" t="s">
+      <c r="B195" s="12" t="s">
         <v>1018</v>
       </c>
       <c r="C195" t="s">
@@ -7361,10 +7370,10 @@
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A196" s="16" t="s">
+      <c r="A196" s="11" t="s">
         <v>1035</v>
       </c>
-      <c r="B196" s="17" t="s">
+      <c r="B196" s="12" t="s">
         <v>1019</v>
       </c>
       <c r="C196" t="s">
@@ -7384,10 +7393,10 @@
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A197" s="16" t="s">
+      <c r="A197" s="11" t="s">
         <v>1036</v>
       </c>
-      <c r="B197" s="17" t="s">
+      <c r="B197" s="12" t="s">
         <v>1020</v>
       </c>
       <c r="C197" t="s">
@@ -7407,10 +7416,10 @@
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A198" s="16" t="s">
+      <c r="A198" s="11" t="s">
         <v>1037</v>
       </c>
-      <c r="B198" s="17" t="s">
+      <c r="B198" s="12" t="s">
         <v>1021</v>
       </c>
       <c r="C198" t="s">
@@ -7430,10 +7439,10 @@
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A199" s="16" t="s">
+      <c r="A199" s="11" t="s">
         <v>1038</v>
       </c>
-      <c r="B199" s="17" t="s">
+      <c r="B199" s="12" t="s">
         <v>1022</v>
       </c>
       <c r="C199" t="s">
@@ -7453,10 +7462,10 @@
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A200" s="16" t="s">
+      <c r="A200" s="11" t="s">
         <v>1039</v>
       </c>
-      <c r="B200" s="17" t="s">
+      <c r="B200" s="12" t="s">
         <v>1030</v>
       </c>
       <c r="C200" t="s">
@@ -7476,10 +7485,10 @@
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A201" s="16" t="s">
+      <c r="A201" s="11" t="s">
         <v>1040</v>
       </c>
-      <c r="B201" s="17" t="s">
+      <c r="B201" s="12" t="s">
         <v>1029</v>
       </c>
       <c r="C201" t="s">
@@ -7499,10 +7508,10 @@
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A202" s="16" t="s">
+      <c r="A202" s="11" t="s">
         <v>1052</v>
       </c>
-      <c r="B202" s="17" t="s">
+      <c r="B202" s="12" t="s">
         <v>1053</v>
       </c>
       <c r="C202" t="s">
@@ -7519,10 +7528,10 @@
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A203" s="16" t="s">
+      <c r="A203" s="11" t="s">
         <v>1058</v>
       </c>
-      <c r="B203" s="17" t="s">
+      <c r="B203" s="12" t="s">
         <v>1056</v>
       </c>
       <c r="C203" t="s">
@@ -7539,10 +7548,10 @@
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A204" s="16" t="s">
+      <c r="A204" s="11" t="s">
         <v>1059</v>
       </c>
-      <c r="B204" s="17" t="s">
+      <c r="B204" s="12" t="s">
         <v>1057</v>
       </c>
       <c r="C204" t="s">
@@ -7559,10 +7568,10 @@
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A205" s="16" t="s">
+      <c r="A205" s="11" t="s">
         <v>1067</v>
       </c>
-      <c r="B205" s="17" t="s">
+      <c r="B205" s="12" t="s">
         <v>1060</v>
       </c>
       <c r="C205" t="s">
@@ -7576,10 +7585,10 @@
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A206" s="16" t="s">
+      <c r="A206" s="11" t="s">
         <v>1068</v>
       </c>
-      <c r="B206" s="17" t="s">
+      <c r="B206" s="12" t="s">
         <v>1061</v>
       </c>
       <c r="C206" t="s">
@@ -7593,10 +7602,10 @@
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A207" s="16" t="s">
+      <c r="A207" s="11" t="s">
         <v>1069</v>
       </c>
-      <c r="B207" s="17" t="s">
+      <c r="B207" s="12" t="s">
         <v>1062</v>
       </c>
       <c r="C207" t="s">
@@ -7610,10 +7619,10 @@
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A208" s="16" t="s">
+      <c r="A208" s="11" t="s">
         <v>1073</v>
       </c>
-      <c r="B208" s="17" t="s">
+      <c r="B208" s="12" t="s">
         <v>1070</v>
       </c>
       <c r="C208" t="s">
@@ -7659,28 +7668,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>567</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="20" t="s">
         <v>650</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="20" t="s">
         <v>651</v>
       </c>
     </row>
@@ -7699,8 +7708,8 @@
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -7818,7 +7827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -7831,24 +7840,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>568</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -7990,10 +7999,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8007,28 +8016,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>569</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="20" t="s">
         <v>650</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="20" t="s">
         <v>651</v>
       </c>
     </row>
@@ -8047,8 +8056,8 @@
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -9456,6 +9465,20 @@
       </c>
       <c r="H95" s="7">
         <v>44932</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E96" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1075</v>
       </c>
     </row>
   </sheetData>
@@ -9475,7 +9498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -9490,28 +9513,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>570</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="20" t="s">
         <v>650</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="20" t="s">
         <v>651</v>
       </c>
     </row>
@@ -9530,8 +9553,8 @@
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -10008,28 +10031,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>571</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="20" t="s">
         <v>650</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="20" t="s">
         <v>651</v>
       </c>
     </row>
@@ -10048,8 +10071,8 @@
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">

</xml_diff>